<commit_message>
Solucionar una problema en el pdf_reader cuando se ententa leer mas de una pagina
</commit_message>
<xml_diff>
--- a/exports/new_export.xlsx
+++ b/exports/new_export.xlsx
@@ -12,6 +12,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pagina2" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pagina3" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pagina4" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pagina5" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1361,4 +1362,220 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Document</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MIL-PRF-19500/426J w/Amendment 2 (Initial Draft) -- Dated 3/31/2023 </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Transistor, PNP, Silicon, Amplifier Type 2N4957, JAN, JANTX, JANTXV, JANS, JANHC, JANKC </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-19500/idprf19500ss426.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MIL-PRF-19500/439J w/Amendment 1 (Initial Draft) -- Dated 4/3/2023 </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Semiconductor Device, Transistor, NPN, Silicon, High-Power, Types 2N5038 and 2N5039, JAN, JANTX, JANTXV, JANS, JANHC, and JANKC </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-19500/idprf19500ss439.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MIL-PRF-19500/782 (Initial Draft) -- Dated 4/3/2023 </t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Transistor, Gallium Nitride, High Electron Mobility Transistor (HEMT), Radiation Hardened, Enhancement Mode, Types 2N7667UFB, 2N7668UFB, 2N7669UFB, Quality Levels JANTXV, JANS JANHC, and JANKC </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-19500/idprf19500ss782.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MIL-PRF-39016/48E -- Dated 3/8/2023 </t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Relays, Electromagnetic, Established Reliability, DPDT, Low Level to 0.5 Ampere (.100 D.I.P. Terminal Spacing), One-Tenth Size, Sensitive, Monostable </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-39016/prf39016ss48.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MIL-PRF-55339/39A w/Amendment 1 -- Dated 2/28/2023 </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Adapter, Connector, Coaxial, Radio Frequency, (Between Series BNC to Series TNC), Class 2, Straight Plug </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-55339/prf55339ss39.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MIL-PRF-55339/48B w/Amendment 2 -- Dated 2/28/2023 </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Adapter, Connector, Coaxial, Radio Frequency, (Between Series SMA to Series TNC), Class 2, Straight Plug </t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-55339/prf55339ss48.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MIL-PRF-55339/51A w/Amendment 1 -- Dated 2/28/2023 </t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Adapter, Connector, Coaxial, Radio Frequency, (Between Series TNC to Series N), Class 2, Straight Plug </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-55339/prf55339ss51.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MIL-PRF-55339/54B w/Amendment 2 -- Dated 2/1/2023 </t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Adapter, Connector, Electrical, Coaxial, Radio Frequency, (Between Series SMA to N) </t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-55339/prf55339ss54.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MIL-PRF-55339/55 w/Amendment 2 -- Dated 2/28/2023 </t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Adapter, Connectors, Electrical, Coaxial, Radio Frequency, Series SMA, Connector Saver </t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-55339/prf55339ss55.pdf</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>